<commit_message>
antes de subir el proyecto a Bitbucket
</commit_message>
<xml_diff>
--- a/Documentacion/Armado de Atributos.xlsx
+++ b/Documentacion/Armado de Atributos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="51">
   <si>
     <t>ResultsComponent</t>
   </si>
@@ -749,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -924,6 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1478,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AH73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="R60" sqref="R60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K32" workbookViewId="0">
+      <selection activeCell="AA56" sqref="AA56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1494,6 +1495,8 @@
     <col min="9" max="9" width="15.6640625" style="4" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" style="4" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="13.5" customWidth="1"/>
+    <col min="28" max="28" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="19" x14ac:dyDescent="0.25">
@@ -2530,30 +2533,18 @@
     <row r="47" spans="2:34" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="G47" s="28"/>
-      <c r="K47" s="5" t="s">
+      <c r="K47" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
-      <c r="O47" s="6"/>
-      <c r="P47" s="7"/>
-      <c r="R47" s="5" t="s">
+      <c r="L47" s="68"/>
+      <c r="R47" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="S47" s="6"/>
-      <c r="T47" s="6"/>
-      <c r="U47" s="6"/>
-      <c r="V47" s="6"/>
-      <c r="W47" s="7"/>
-      <c r="AA47" s="5" t="s">
+      <c r="S47" s="68"/>
+      <c r="AA47" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="AB47" s="6"/>
-      <c r="AC47" s="6"/>
-      <c r="AD47" s="6"/>
-      <c r="AE47" s="6"/>
-      <c r="AF47" s="7"/>
+      <c r="AB47" s="68"/>
     </row>
     <row r="48" spans="2:34" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
@@ -2569,59 +2560,23 @@
       <c r="K48" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="L48" s="39" t="s">
+      <c r="L48" s="41" t="s">
         <v>18</v>
-      </c>
-      <c r="M48" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="N48" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="O48" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="P48" s="41" t="s">
-        <v>21</v>
       </c>
       <c r="R48" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="S48" s="39" t="s">
+      <c r="S48" s="41" t="s">
         <v>18</v>
-      </c>
-      <c r="T48" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="U48" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="V48" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="W48" s="41" t="s">
-        <v>21</v>
       </c>
       <c r="AA48" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AB48" s="39" t="s">
+      <c r="AB48" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="AC48" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD48" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE48" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF48" s="41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="2:32" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:28" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="D49" s="46" t="s">
         <v>33</v>
@@ -2632,62 +2587,20 @@
       <c r="H49" s="4"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
-      <c r="K49" s="43">
-        <v>15</v>
-      </c>
-      <c r="L49" s="25">
+      <c r="K49" s="43"/>
+      <c r="L49" s="67">
         <v>4</v>
       </c>
-      <c r="M49" s="25">
+      <c r="R49" s="43"/>
+      <c r="S49" s="67">
+        <v>4</v>
+      </c>
+      <c r="AA49" s="56"/>
+      <c r="AB49" s="65">
         <v>2</v>
       </c>
-      <c r="N49" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="O49" s="25">
-        <v>9</v>
-      </c>
-      <c r="P49" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="R49" s="43">
-        <v>15</v>
-      </c>
-      <c r="S49" s="25">
-        <v>4</v>
-      </c>
-      <c r="T49" s="25">
-        <v>2</v>
-      </c>
-      <c r="U49" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="V49" s="25">
-        <v>9</v>
-      </c>
-      <c r="W49" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA49" s="56">
-        <v>2</v>
-      </c>
-      <c r="AB49" s="64">
-        <v>2</v>
-      </c>
-      <c r="AC49" s="64">
-        <v>1</v>
-      </c>
-      <c r="AD49" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE49" s="64">
-        <v>1</v>
-      </c>
-      <c r="AF49" s="65" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="2:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="D50" s="49" t="s">
         <v>19</v>
@@ -2704,28 +2617,12 @@
       <c r="H50" s="4"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="AA50" s="42">
+      <c r="AA50" s="42"/>
+      <c r="AB50" s="60">
         <v>4</v>
       </c>
-      <c r="AB50" s="59">
-        <v>4</v>
-      </c>
-      <c r="AC50" s="59">
-        <v>1</v>
-      </c>
-      <c r="AD50" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE50" s="59">
-        <v>1</v>
-      </c>
-      <c r="AF50" s="60" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="2:32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B51" s="2"/>
       <c r="D51" s="42">
         <v>1</v>
@@ -2742,28 +2639,12 @@
       <c r="H51" s="4"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="AA51" s="42">
+      <c r="AA51" s="42"/>
+      <c r="AB51" s="60">
         <v>5</v>
       </c>
-      <c r="AB51" s="59">
-        <v>5</v>
-      </c>
-      <c r="AC51" s="59">
-        <v>1</v>
-      </c>
-      <c r="AD51" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE51" s="59">
-        <v>1</v>
-      </c>
-      <c r="AF51" s="60" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="2:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="D52" s="42">
         <v>1</v>
@@ -2780,26 +2661,12 @@
       <c r="H52" s="4"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
-      <c r="AA52" s="43">
+      <c r="AA52" s="43"/>
+      <c r="AB52" s="67">
         <v>6</v>
       </c>
-      <c r="AB52" s="66">
-        <v>6</v>
-      </c>
-      <c r="AC52" s="66">
-        <v>1</v>
-      </c>
-      <c r="AD52" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE52" s="66">
-        <v>1</v>
-      </c>
-      <c r="AF52" s="67" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="2:32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="D53" s="42">
         <v>1</v>
@@ -2817,7 +2684,7 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:28" x14ac:dyDescent="0.2">
       <c r="D54" s="50">
         <v>2</v>
       </c>
@@ -2837,7 +2704,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:28" x14ac:dyDescent="0.2">
       <c r="D55" s="50">
         <v>2</v>
       </c>
@@ -2851,7 +2718,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:28" x14ac:dyDescent="0.2">
       <c r="D56" s="50">
         <v>2</v>
       </c>
@@ -2871,7 +2738,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:28" x14ac:dyDescent="0.2">
       <c r="D57" s="50">
         <v>2</v>
       </c>
@@ -2891,7 +2758,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:28" x14ac:dyDescent="0.2">
       <c r="D58" s="50">
         <v>2</v>
       </c>
@@ -2905,7 +2772,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="2:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D59" s="53">
         <v>2</v>
       </c>
@@ -2922,16 +2789,16 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:28" x14ac:dyDescent="0.2">
       <c r="R60" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="2:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="G62" s="28"/>
     </row>
-    <row r="63" spans="2:32" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:28" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="2"/>
       <c r="D63" s="5" t="s">
         <v>35</v>
@@ -2947,7 +2814,7 @@
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="2:32" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:28" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="D64" s="46" t="s">
         <v>37</v>
@@ -3137,15 +3004,12 @@
       <c r="J73" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="17">
     <mergeCell ref="I63:L63"/>
     <mergeCell ref="R32:W32"/>
     <mergeCell ref="R40:W40"/>
     <mergeCell ref="AA32:AF32"/>
     <mergeCell ref="AA40:AF40"/>
-    <mergeCell ref="AA47:AF47"/>
-    <mergeCell ref="R47:W47"/>
-    <mergeCell ref="K47:P47"/>
     <mergeCell ref="C31:H31"/>
     <mergeCell ref="D49:G49"/>
     <mergeCell ref="D63:G63"/>

</xml_diff>